<commit_message>
11/09: First CE modelling attempts.
</commit_message>
<xml_diff>
--- a/Data/Pilot1/D2_Pilot1_Covariates.xlsx
+++ b/Data/Pilot1/D2_Pilot1_Covariates.xlsx
@@ -5,17 +5,20 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://leeds365-my.sharepoint.com/personal/earpkin_leeds_ac_uk/Documents/DRUID/D2/Data/Pilot1/delivery/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://leeds365-my.sharepoint.com/personal/earpkin_leeds_ac_uk/Documents/DRUID/D2/Analysis/D2Backup/Data/Pilot1/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="3" documentId="13_ncr:1_{2828253C-1F41-4EB5-B00E-51F8E11681DC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B0D1241C-6033-453E-96B4-31375FDCE7EF}"/>
+  <xr:revisionPtr revIDLastSave="15" documentId="13_ncr:1_{2828253C-1F41-4EB5-B00E-51F8E11681DC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{CA292D8E-DD73-4FE2-B65E-5CAB0968220D}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
     <sheet name="Dictionary" sheetId="2" r:id="rId2"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Data!$BP$1:$BT$51</definedName>
+  </definedNames>
   <calcPr calcId="0"/>
 </workbook>
 </file>
@@ -9551,8 +9554,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:FC51"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="T9" sqref="T9"/>
+    <sheetView topLeftCell="EW1" workbookViewId="0">
+      <selection activeCell="EZ1" sqref="EZ1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.453125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -9560,6 +9563,7 @@
     <col min="3" max="3" width="18.26953125" bestFit="1" customWidth="1"/>
     <col min="16" max="17" width="14.90625" bestFit="1" customWidth="1"/>
     <col min="18" max="20" width="17.36328125" bestFit="1" customWidth="1"/>
+    <col min="30" max="35" width="20.1796875" bestFit="1" customWidth="1"/>
     <col min="159" max="159" width="30.90625" customWidth="1"/>
   </cols>
   <sheetData>
@@ -33048,6 +33052,7 @@
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="BP1:BT51" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
@@ -33057,8 +33062,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:D557"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+    <sheetView tabSelected="1" topLeftCell="A254" workbookViewId="0">
+      <selection activeCell="J266" sqref="J266"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.453125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>